<commit_message>
funds and source file checked
</commit_message>
<xml_diff>
--- a/data/funds_ab_in_2023.xlsx
+++ b/data/funds_ab_in_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleaw\OneDrive\Documents\PhD Fall 2021 - Spring 2022\Merriman RA\Fiscal Futures IGPA\Fiscal-Future-Topics\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474E7C05-E0D0-4674-AB6E-5196F9C468F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E0FA4D-E587-4D50-9996-09678C78977E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="9030" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -7911,7 +7911,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -7961,12 +7961,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8026,7 +8020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -8043,39 +8037,18 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8191,21 +8164,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92861C71-2608-406B-AB38-61A950AD4A6E}" name="Table1" displayName="Table1" ref="A1:I1130" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92861C71-2608-406B-AB38-61A950AD4A6E}" name="Table1" displayName="Table1" ref="A1:I1130" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:I1130" xr:uid="{92861C71-2608-406B-AB38-61A950AD4A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I1130">
     <sortCondition ref="A1:A1130"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5C12AE88-F5C0-4F1D-BC84-FFCA81419500}" name="fund" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{CEDB1617-12CC-4191-B126-9922068A1353}" name="fund_ab" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{4C1E1072-690E-4905-AD33-33117D00B670}" name="fund_ioc" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{57A480F5-EA3F-465F-975E-2A2B1C7302FA}" name="fund_re" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{5C244DC3-32C4-4224-BC6D-7AE06CED4898}" name="a_end" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{8464D253-7DFF-48A9-878F-3C3F48DA8414}" name="in_ff" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{ECBCF6D7-D1E8-4215-AAC1-21E353589401}" name="fund_name_ab" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{43B46110-966C-42D4-BE04-99C9CB9FACD9}" name="fund_category" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{DAF8ADA5-8C0F-4603-BF33-F6FD7A1BE6F8}" name="fund_cat_name" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5C12AE88-F5C0-4F1D-BC84-FFCA81419500}" name="fund" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{CEDB1617-12CC-4191-B126-9922068A1353}" name="fund_ab" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{4C1E1072-690E-4905-AD33-33117D00B670}" name="fund_ioc" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{57A480F5-EA3F-465F-975E-2A2B1C7302FA}" name="fund_re" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{5C244DC3-32C4-4224-BC6D-7AE06CED4898}" name="a_end" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{8464D253-7DFF-48A9-878F-3C3F48DA8414}" name="in_ff" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{ECBCF6D7-D1E8-4215-AAC1-21E353589401}" name="fund_name_ab" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{43B46110-966C-42D4-BE04-99C9CB9FACD9}" name="fund_category" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{DAF8ADA5-8C0F-4603-BF33-F6FD7A1BE6F8}" name="fund_cat_name" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8537,7 +8510,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="G665" sqref="G665"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8760,7 +8733,7 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="1" t="s">
         <v>1241</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -9246,7 +9219,7 @@
       <c r="F26" s="1">
         <v>1</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="1" t="s">
         <v>1259</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -10272,7 +10245,7 @@
       <c r="F64" s="1">
         <v>1</v>
       </c>
-      <c r="G64" s="14" t="s">
+      <c r="G64" s="1" t="s">
         <v>1297</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -10299,7 +10272,7 @@
       <c r="F65" s="1">
         <v>1</v>
       </c>
-      <c r="G65" s="14" t="s">
+      <c r="G65" s="1" t="s">
         <v>1298</v>
       </c>
       <c r="H65" s="1" t="s">
@@ -10326,7 +10299,7 @@
       <c r="F66" s="1">
         <v>1</v>
       </c>
-      <c r="G66" s="14" t="s">
+      <c r="G66" s="1" t="s">
         <v>1299</v>
       </c>
       <c r="H66" s="1" t="s">
@@ -10380,7 +10353,7 @@
       <c r="F68" s="1">
         <v>1</v>
       </c>
-      <c r="G68" s="14" t="s">
+      <c r="G68" s="1" t="s">
         <v>1301</v>
       </c>
       <c r="H68" s="1" t="s">
@@ -10407,7 +10380,7 @@
       <c r="F69" s="1">
         <v>1</v>
       </c>
-      <c r="G69" s="14" t="s">
+      <c r="G69" s="1" t="s">
         <v>1302</v>
       </c>
       <c r="H69" s="1" t="s">
@@ -10839,7 +10812,7 @@
       <c r="F85" s="1">
         <v>1</v>
       </c>
-      <c r="G85" s="14" t="s">
+      <c r="G85" s="1" t="s">
         <v>1318</v>
       </c>
       <c r="H85" s="1" t="s">
@@ -10985,23 +10958,23 @@
       </c>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="2" t="s">
         <v>2573</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D91" s="17" t="s">
+      <c r="D91" s="2" t="s">
         <v>2310</v>
       </c>
-      <c r="E91" s="17"/>
-      <c r="F91" s="17" t="s">
+      <c r="E91" s="2"/>
+      <c r="F91" s="2" t="s">
         <v>2313</v>
       </c>
-      <c r="G91" s="17" t="s">
+      <c r="G91" s="2" t="s">
         <v>2570</v>
       </c>
       <c r="H91" s="2" t="s">
@@ -11028,7 +11001,7 @@
       <c r="F92" s="1">
         <v>1</v>
       </c>
-      <c r="G92" s="14" t="s">
+      <c r="G92" s="1" t="s">
         <v>1325</v>
       </c>
       <c r="H92" s="1" t="s">
@@ -11055,7 +11028,7 @@
       <c r="F93" s="1">
         <v>1</v>
       </c>
-      <c r="G93" s="14" t="s">
+      <c r="G93" s="1" t="s">
         <v>1326</v>
       </c>
       <c r="H93" s="1" t="s">
@@ -11082,7 +11055,7 @@
       <c r="F94" s="1">
         <v>1</v>
       </c>
-      <c r="G94" s="14" t="s">
+      <c r="G94" s="1" t="s">
         <v>1327</v>
       </c>
       <c r="H94" s="1" t="s">
@@ -11298,7 +11271,7 @@
       <c r="F102" s="1">
         <v>1</v>
       </c>
-      <c r="G102" s="18" t="s">
+      <c r="G102" s="15" t="s">
         <v>2444</v>
       </c>
       <c r="H102" s="1" t="s">
@@ -12159,7 +12132,7 @@
       <c r="F134" s="1">
         <v>1</v>
       </c>
-      <c r="G134" s="14" t="s">
+      <c r="G134" s="1" t="s">
         <v>1367</v>
       </c>
       <c r="H134" s="1" t="s">
@@ -12429,7 +12402,7 @@
       <c r="F144" s="1">
         <v>1</v>
       </c>
-      <c r="G144" s="14" t="s">
+      <c r="G144" s="1" t="s">
         <v>1377</v>
       </c>
       <c r="H144" s="1" t="s">
@@ -12564,7 +12537,7 @@
       <c r="F149" s="1">
         <v>1</v>
       </c>
-      <c r="G149" s="14" t="s">
+      <c r="G149" s="1" t="s">
         <v>1382</v>
       </c>
       <c r="H149" s="1" t="s">
@@ -12763,7 +12736,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" ht="28.5">
       <c r="A157" s="1" t="s">
         <v>156</v>
       </c>
@@ -12942,7 +12915,7 @@
       <c r="F163" s="1">
         <v>1</v>
       </c>
-      <c r="G163" s="14" t="s">
+      <c r="G163" s="1" t="s">
         <v>1396</v>
       </c>
       <c r="H163" s="1" t="s">
@@ -12996,7 +12969,7 @@
       <c r="F165" s="1">
         <v>1</v>
       </c>
-      <c r="G165" s="14" t="s">
+      <c r="G165" s="1" t="s">
         <v>1398</v>
       </c>
       <c r="H165" s="1" t="s">
@@ -13168,7 +13141,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" ht="15.3">
       <c r="A172" s="10" t="s">
         <v>2512</v>
       </c>
@@ -13401,7 +13374,7 @@
       <c r="F180" s="1">
         <v>1</v>
       </c>
-      <c r="G180" s="14" t="s">
+      <c r="G180" s="1" t="s">
         <v>1411</v>
       </c>
       <c r="H180" s="1" t="s">
@@ -13600,7 +13573,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="28.5">
+    <row r="188" spans="1:9">
       <c r="A188" s="1" t="s">
         <v>185</v>
       </c>
@@ -13725,7 +13698,7 @@
       <c r="F192" s="1">
         <v>0</v>
       </c>
-      <c r="G192" s="14" t="s">
+      <c r="G192" s="1" t="s">
         <v>1423</v>
       </c>
       <c r="H192" s="1" t="s">
@@ -13779,7 +13752,7 @@
       <c r="F194" s="1">
         <v>0</v>
       </c>
-      <c r="G194" s="14" t="s">
+      <c r="G194" s="1" t="s">
         <v>1425</v>
       </c>
       <c r="H194" s="1" t="s">
@@ -13968,7 +13941,7 @@
       <c r="F201" s="1">
         <v>1</v>
       </c>
-      <c r="G201" s="14" t="s">
+      <c r="G201" s="1" t="s">
         <v>1432</v>
       </c>
       <c r="H201" s="1" t="s">
@@ -13995,7 +13968,7 @@
       <c r="F202" s="2" t="s">
         <v>2313</v>
       </c>
-      <c r="G202" s="14" t="s">
+      <c r="G202" s="1" t="s">
         <v>2529</v>
       </c>
       <c r="H202" s="2" t="s">
@@ -14113,7 +14086,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="15.3">
+    <row r="207" spans="1:9">
       <c r="A207" s="1" t="s">
         <v>204</v>
       </c>
@@ -14184,7 +14157,7 @@
       <c r="F209" s="1">
         <v>1</v>
       </c>
-      <c r="G209" s="14" t="s">
+      <c r="G209" s="1" t="s">
         <v>1440</v>
       </c>
       <c r="H209" s="1" t="s">
@@ -14248,7 +14221,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" ht="15.3">
       <c r="A212" s="13" t="s">
         <v>2513</v>
       </c>
@@ -14265,7 +14238,7 @@
       <c r="F212" s="2" t="s">
         <v>2313</v>
       </c>
-      <c r="G212" s="22" t="s">
+      <c r="G212" s="13" t="s">
         <v>2508</v>
       </c>
       <c r="H212" s="2" t="s">
@@ -14670,7 +14643,7 @@
       <c r="F227" s="1">
         <v>1</v>
       </c>
-      <c r="G227" s="14" t="s">
+      <c r="G227" s="1" t="s">
         <v>1457</v>
       </c>
       <c r="H227" s="1" t="s">
@@ -14940,7 +14913,7 @@
       <c r="F237" s="1">
         <v>1</v>
       </c>
-      <c r="G237" s="14" t="s">
+      <c r="G237" s="1" t="s">
         <v>1468</v>
       </c>
       <c r="H237" s="1" t="s">
@@ -14994,7 +14967,7 @@
       <c r="F239" s="1">
         <v>1</v>
       </c>
-      <c r="G239" s="14" t="s">
+      <c r="G239" s="1" t="s">
         <v>1470</v>
       </c>
       <c r="H239" s="1" t="s">
@@ -15102,7 +15075,7 @@
       <c r="F243" s="1">
         <v>1</v>
       </c>
-      <c r="G243" s="19" t="s">
+      <c r="G243" s="16" t="s">
         <v>2406</v>
       </c>
       <c r="H243" s="1" t="s">
@@ -15345,7 +15318,7 @@
       <c r="F252" s="2" t="s">
         <v>2313</v>
       </c>
-      <c r="G252" s="20" t="s">
+      <c r="G252" s="2" t="s">
         <v>2545</v>
       </c>
       <c r="H252" s="2" t="s">
@@ -15399,7 +15372,7 @@
       <c r="F254" s="1">
         <v>1</v>
       </c>
-      <c r="G254" s="14" t="s">
+      <c r="G254" s="1" t="s">
         <v>1485</v>
       </c>
       <c r="H254" s="1" t="s">
@@ -15463,7 +15436,7 @@
         <v>2287</v>
       </c>
     </row>
-    <row r="257" spans="1:9" ht="15.3">
+    <row r="257" spans="1:9">
       <c r="A257" s="1" t="s">
         <v>254</v>
       </c>
@@ -15507,7 +15480,7 @@
       <c r="F258" s="1">
         <v>0</v>
       </c>
-      <c r="G258" s="14" t="s">
+      <c r="G258" s="1" t="s">
         <v>1489</v>
       </c>
       <c r="H258" s="1" t="s">
@@ -15588,7 +15561,7 @@
       <c r="F261" s="1">
         <v>0</v>
       </c>
-      <c r="G261" s="14" t="s">
+      <c r="G261" s="1" t="s">
         <v>1492</v>
       </c>
       <c r="H261" s="1" t="s">
@@ -15804,7 +15777,7 @@
       <c r="F269" s="1">
         <v>1</v>
       </c>
-      <c r="G269" s="14" t="s">
+      <c r="G269" s="1" t="s">
         <v>1500</v>
       </c>
       <c r="H269" s="1" t="s">
@@ -16155,7 +16128,7 @@
       <c r="F282" s="1">
         <v>0</v>
       </c>
-      <c r="G282" s="14" t="s">
+      <c r="G282" s="1" t="s">
         <v>1513</v>
       </c>
       <c r="H282" s="1" t="s">
@@ -16317,7 +16290,7 @@
       <c r="F288" s="1">
         <v>1</v>
       </c>
-      <c r="G288" s="14" t="s">
+      <c r="G288" s="1" t="s">
         <v>1519</v>
       </c>
       <c r="H288" s="1" t="s">
@@ -16371,7 +16344,7 @@
       <c r="F290" s="1">
         <v>1</v>
       </c>
-      <c r="G290" s="14" t="s">
+      <c r="G290" s="1" t="s">
         <v>1521</v>
       </c>
       <c r="H290" s="1" t="s">
@@ -16587,7 +16560,7 @@
       <c r="F298" s="2" t="s">
         <v>2313</v>
       </c>
-      <c r="G298" s="20" t="s">
+      <c r="G298" s="2" t="s">
         <v>2549</v>
       </c>
       <c r="H298" s="2" t="s">
@@ -16668,7 +16641,7 @@
       <c r="F301" s="1">
         <v>1</v>
       </c>
-      <c r="G301" s="14" t="s">
+      <c r="G301" s="1" t="s">
         <v>1532</v>
       </c>
       <c r="H301" s="1" t="s">
@@ -16776,7 +16749,7 @@
       <c r="F305" s="1">
         <v>1</v>
       </c>
-      <c r="G305" s="14" t="s">
+      <c r="G305" s="1" t="s">
         <v>1536</v>
       </c>
       <c r="H305" s="1" t="s">
@@ -17262,7 +17235,7 @@
       <c r="F323" s="1">
         <v>1</v>
       </c>
-      <c r="G323" s="14" t="s">
+      <c r="G323" s="1" t="s">
         <v>1553</v>
       </c>
       <c r="H323" s="1" t="s">
@@ -17316,7 +17289,7 @@
       <c r="F325" s="1">
         <v>1</v>
       </c>
-      <c r="G325" s="14" t="s">
+      <c r="G325" s="1" t="s">
         <v>1555</v>
       </c>
       <c r="H325" s="1" t="s">
@@ -17586,7 +17559,7 @@
       <c r="F335" s="1">
         <v>1</v>
       </c>
-      <c r="G335" s="14" t="s">
+      <c r="G335" s="1" t="s">
         <v>2412</v>
       </c>
       <c r="H335" s="1" t="s">
@@ -17893,7 +17866,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="347" spans="1:9" ht="15.3">
+    <row r="347" spans="1:9">
       <c r="A347" s="1" t="s">
         <v>343</v>
       </c>
@@ -17991,7 +17964,7 @@
       <c r="F350" s="1">
         <v>0</v>
       </c>
-      <c r="G350" s="14" t="s">
+      <c r="G350" s="1" t="s">
         <v>1580</v>
       </c>
       <c r="H350" s="1" t="s">
@@ -18315,7 +18288,7 @@
       <c r="F362" s="1">
         <v>1</v>
       </c>
-      <c r="G362" s="14" t="s">
+      <c r="G362" s="1" t="s">
         <v>1592</v>
       </c>
       <c r="H362" s="1" t="s">
@@ -18541,7 +18514,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="371" spans="1:9">
+    <row r="371" spans="1:9" ht="15.3">
       <c r="A371" s="13" t="s">
         <v>2514</v>
       </c>
@@ -19648,7 +19621,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="412" spans="1:9">
+    <row r="412" spans="1:9" ht="15.3">
       <c r="A412" s="10" t="s">
         <v>2515</v>
       </c>
@@ -19800,7 +19773,7 @@
       <c r="F417" s="1">
         <v>1</v>
       </c>
-      <c r="G417" s="14" t="s">
+      <c r="G417" s="1" t="s">
         <v>1643</v>
       </c>
       <c r="H417" s="1" t="s">
@@ -20016,7 +19989,7 @@
       <c r="F425" s="1">
         <v>1</v>
       </c>
-      <c r="G425" s="14" t="s">
+      <c r="G425" s="1" t="s">
         <v>1651</v>
       </c>
       <c r="H425" s="1" t="s">
@@ -20053,7 +20026,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="427" spans="1:9">
+    <row r="427" spans="1:9" ht="15.3">
       <c r="A427" s="13" t="s">
         <v>2516</v>
       </c>
@@ -20421,7 +20394,7 @@
       <c r="F440" s="1">
         <v>1</v>
       </c>
-      <c r="G440" s="14" t="s">
+      <c r="G440" s="1" t="s">
         <v>1665</v>
       </c>
       <c r="H440" s="1" t="s">
@@ -20566,7 +20539,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="446" spans="1:9" ht="15.3">
+    <row r="446" spans="1:9">
       <c r="A446" s="1" t="s">
         <v>437</v>
       </c>
@@ -20610,7 +20583,7 @@
       <c r="F447" s="1">
         <v>0</v>
       </c>
-      <c r="G447" s="14" t="s">
+      <c r="G447" s="1" t="s">
         <v>1672</v>
       </c>
       <c r="H447" s="1" t="s">
@@ -20880,7 +20853,7 @@
       <c r="F457" s="1">
         <v>1</v>
       </c>
-      <c r="G457" s="14" t="s">
+      <c r="G457" s="1" t="s">
         <v>1682</v>
       </c>
       <c r="H457" s="1" t="s">
@@ -21312,7 +21285,7 @@
       <c r="F473" s="1">
         <v>1</v>
       </c>
-      <c r="G473" s="14" t="s">
+      <c r="G473" s="1" t="s">
         <v>1698</v>
       </c>
       <c r="H473" s="1" t="s">
@@ -21376,7 +21349,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="476" spans="1:9" ht="15.3">
+    <row r="476" spans="1:9">
       <c r="A476" s="1" t="s">
         <v>467</v>
       </c>
@@ -21835,7 +21808,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="493" spans="1:9" ht="15.3">
+    <row r="493" spans="1:9">
       <c r="A493" s="1" t="s">
         <v>484</v>
       </c>
@@ -22095,7 +22068,7 @@
       <c r="F502" s="1">
         <v>1</v>
       </c>
-      <c r="G502" s="14" t="s">
+      <c r="G502" s="1" t="s">
         <v>1727</v>
       </c>
       <c r="H502" s="1" t="s">
@@ -22240,7 +22213,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="508" spans="1:9" ht="15.3">
+    <row r="508" spans="1:9">
       <c r="A508" s="1" t="s">
         <v>499</v>
       </c>
@@ -22321,7 +22294,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="511" spans="1:9" ht="15.3">
+    <row r="511" spans="1:9">
       <c r="A511" s="1" t="s">
         <v>502</v>
       </c>
@@ -22554,7 +22527,7 @@
       <c r="F519" s="1">
         <v>1</v>
       </c>
-      <c r="G519" s="14" t="s">
+      <c r="G519" s="1" t="s">
         <v>1744</v>
       </c>
       <c r="H519" s="1" t="s">
@@ -22878,7 +22851,7 @@
       <c r="F531" s="1">
         <v>1</v>
       </c>
-      <c r="G531" s="14" t="s">
+      <c r="G531" s="1" t="s">
         <v>1756</v>
       </c>
       <c r="H531" s="1" t="s">
@@ -23418,7 +23391,7 @@
       <c r="F551" s="1">
         <v>1</v>
       </c>
-      <c r="G551" s="14" t="s">
+      <c r="G551" s="1" t="s">
         <v>1776</v>
       </c>
       <c r="H551" s="1" t="s">
@@ -23823,7 +23796,7 @@
       <c r="F566" s="1">
         <v>1</v>
       </c>
-      <c r="G566" s="14" t="s">
+      <c r="G566" s="1" t="s">
         <v>1791</v>
       </c>
       <c r="H566" s="1" t="s">
@@ -24039,7 +24012,7 @@
       <c r="F574" s="1">
         <v>1</v>
       </c>
-      <c r="G574" s="14" t="s">
+      <c r="G574" s="1" t="s">
         <v>1799</v>
       </c>
       <c r="H574" s="1" t="s">
@@ -24093,7 +24066,7 @@
       <c r="F576" s="1">
         <v>1</v>
       </c>
-      <c r="G576" s="14" t="s">
+      <c r="G576" s="1" t="s">
         <v>1801</v>
       </c>
       <c r="H576" s="1" t="s">
@@ -24606,7 +24579,7 @@
       <c r="F595" s="1">
         <v>1</v>
       </c>
-      <c r="G595" s="14" t="s">
+      <c r="G595" s="1" t="s">
         <v>1818</v>
       </c>
       <c r="H595" s="1" t="s">
@@ -24660,7 +24633,7 @@
       <c r="F597" s="1">
         <v>1</v>
       </c>
-      <c r="G597" s="14" t="s">
+      <c r="G597" s="1" t="s">
         <v>1820</v>
       </c>
       <c r="H597" s="1" t="s">
@@ -25065,7 +25038,7 @@
       <c r="F612" s="1">
         <v>1</v>
       </c>
-      <c r="G612" s="14" t="s">
+      <c r="G612" s="1" t="s">
         <v>1835</v>
       </c>
       <c r="H612" s="1" t="s">
@@ -25092,7 +25065,7 @@
       <c r="F613" s="1">
         <v>1</v>
       </c>
-      <c r="G613" s="14" t="s">
+      <c r="G613" s="1" t="s">
         <v>1836</v>
       </c>
       <c r="H613" s="1" t="s">
@@ -25333,7 +25306,7 @@
       <c r="F622" s="1">
         <v>1</v>
       </c>
-      <c r="G622" s="14" t="s">
+      <c r="G622" s="1" t="s">
         <v>1845</v>
       </c>
       <c r="H622" s="1" t="s">
@@ -25549,7 +25522,7 @@
       <c r="F630" s="1">
         <v>1</v>
       </c>
-      <c r="G630" s="14" t="s">
+      <c r="G630" s="1" t="s">
         <v>1853</v>
       </c>
       <c r="H630" s="1" t="s">
@@ -25603,7 +25576,7 @@
       <c r="F632" s="1">
         <v>0</v>
       </c>
-      <c r="G632" s="14" t="s">
+      <c r="G632" s="1" t="s">
         <v>1855</v>
       </c>
       <c r="H632" s="1" t="s">
@@ -25711,7 +25684,7 @@
       <c r="F636" s="1">
         <v>1</v>
       </c>
-      <c r="G636" s="14" t="s">
+      <c r="G636" s="1" t="s">
         <v>1859</v>
       </c>
       <c r="H636" s="1" t="s">
@@ -26143,7 +26116,7 @@
       <c r="F652" s="1">
         <v>1</v>
       </c>
-      <c r="G652" s="14" t="s">
+      <c r="G652" s="1" t="s">
         <v>1875</v>
       </c>
       <c r="H652" s="1" t="s">
@@ -26359,7 +26332,7 @@
       <c r="F660" s="1">
         <v>1</v>
       </c>
-      <c r="G660" s="14" t="s">
+      <c r="G660" s="1" t="s">
         <v>1883</v>
       </c>
       <c r="H660" s="1" t="s">
@@ -28006,7 +27979,7 @@
       <c r="F721" s="1">
         <v>1</v>
       </c>
-      <c r="G721" s="14" t="s">
+      <c r="G721" s="1" t="s">
         <v>1944</v>
       </c>
       <c r="H721" s="1" t="s">
@@ -28114,7 +28087,7 @@
       <c r="F725" s="1">
         <v>1</v>
       </c>
-      <c r="G725" s="18" t="s">
+      <c r="G725" s="15" t="s">
         <v>2499</v>
       </c>
       <c r="H725" s="1" t="s">
@@ -28571,7 +28544,7 @@
       <c r="F742" s="1">
         <v>1</v>
       </c>
-      <c r="G742" s="14" t="s">
+      <c r="G742" s="1" t="s">
         <v>1965</v>
       </c>
       <c r="H742" s="1" t="s">
@@ -28652,7 +28625,7 @@
       <c r="F745" s="1">
         <v>1</v>
       </c>
-      <c r="G745" s="14" t="s">
+      <c r="G745" s="1" t="s">
         <v>1968</v>
       </c>
       <c r="H745" s="1" t="s">
@@ -28733,7 +28706,7 @@
       <c r="F748" s="1">
         <v>1</v>
       </c>
-      <c r="G748" s="15" t="s">
+      <c r="G748" s="14" t="s">
         <v>2306</v>
       </c>
       <c r="H748" s="1" t="s">
@@ -29084,7 +29057,7 @@
       <c r="F761" s="1">
         <v>1</v>
       </c>
-      <c r="G761" s="14" t="s">
+      <c r="G761" s="1" t="s">
         <v>1984</v>
       </c>
       <c r="H761" s="1" t="s">
@@ -29392,29 +29365,29 @@
       </c>
     </row>
     <row r="773" spans="1:9">
-      <c r="A773" s="17" t="s">
+      <c r="A773" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="B773" s="17" t="s">
+      <c r="B773" s="2" t="s">
         <v>2565</v>
       </c>
-      <c r="C773" s="17" t="s">
+      <c r="C773" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="D773" s="17" t="s">
+      <c r="D773" s="2" t="s">
         <v>2310</v>
       </c>
-      <c r="E773" s="17"/>
-      <c r="F773" s="17" t="s">
+      <c r="E773" s="2"/>
+      <c r="F773" s="2" t="s">
         <v>2313</v>
       </c>
-      <c r="G773" s="21" t="s">
+      <c r="G773" s="17" t="s">
         <v>2524</v>
       </c>
-      <c r="H773" s="17" t="s">
-        <v>2278</v>
-      </c>
-      <c r="I773" s="17" t="s">
+      <c r="H773" s="2" t="s">
+        <v>2278</v>
+      </c>
+      <c r="I773" s="2" t="s">
         <v>2593</v>
       </c>
     </row>
@@ -29570,7 +29543,7 @@
       <c r="F779" s="1">
         <v>1</v>
       </c>
-      <c r="G779" s="14" t="s">
+      <c r="G779" s="1" t="s">
         <v>2002</v>
       </c>
       <c r="H779" s="1" t="s">
@@ -29759,7 +29732,7 @@
       <c r="F786" s="1">
         <v>1</v>
       </c>
-      <c r="G786" s="14" t="s">
+      <c r="G786" s="1" t="s">
         <v>2009</v>
       </c>
       <c r="H786" s="1" t="s">
@@ -29813,7 +29786,7 @@
       <c r="F788" s="1">
         <v>1</v>
       </c>
-      <c r="G788" s="14" t="s">
+      <c r="G788" s="1" t="s">
         <v>2011</v>
       </c>
       <c r="H788" s="1" t="s">
@@ -29894,7 +29867,7 @@
       <c r="F791" s="1">
         <v>0</v>
       </c>
-      <c r="G791" s="14" t="s">
+      <c r="G791" s="1" t="s">
         <v>2014</v>
       </c>
       <c r="H791" s="1" t="s">
@@ -30083,7 +30056,7 @@
       <c r="F798" s="1">
         <v>1</v>
       </c>
-      <c r="G798" s="14" t="s">
+      <c r="G798" s="1" t="s">
         <v>2021</v>
       </c>
       <c r="H798" s="1" t="s">
@@ -30326,7 +30299,7 @@
       <c r="F807" s="1" t="s">
         <v>2313</v>
       </c>
-      <c r="G807" s="14" t="s">
+      <c r="G807" s="1" t="s">
         <v>2030</v>
       </c>
       <c r="H807" s="1" t="s">
@@ -30407,7 +30380,7 @@
       <c r="F810" s="1">
         <v>1</v>
       </c>
-      <c r="G810" s="14" t="s">
+      <c r="G810" s="1" t="s">
         <v>2033</v>
       </c>
       <c r="H810" s="1" t="s">
@@ -30461,7 +30434,7 @@
       <c r="F812" s="1">
         <v>1</v>
       </c>
-      <c r="G812" s="14" t="s">
+      <c r="G812" s="1" t="s">
         <v>2035</v>
       </c>
       <c r="H812" s="1" t="s">
@@ -30542,7 +30515,7 @@
       <c r="F815" s="1">
         <v>1</v>
       </c>
-      <c r="G815" s="14" t="s">
+      <c r="G815" s="1" t="s">
         <v>2038</v>
       </c>
       <c r="H815" s="1" t="s">
@@ -30569,7 +30542,7 @@
       <c r="F816" s="1">
         <v>1</v>
       </c>
-      <c r="G816" s="14" t="s">
+      <c r="G816" s="1" t="s">
         <v>2039</v>
       </c>
       <c r="H816" s="1" t="s">
@@ -30623,7 +30596,7 @@
       <c r="F818" s="1">
         <v>1</v>
       </c>
-      <c r="G818" s="14" t="s">
+      <c r="G818" s="1" t="s">
         <v>2041</v>
       </c>
       <c r="H818" s="1" t="s">
@@ -30650,7 +30623,7 @@
       <c r="F819" s="1">
         <v>1</v>
       </c>
-      <c r="G819" s="14" t="s">
+      <c r="G819" s="1" t="s">
         <v>2042</v>
       </c>
       <c r="H819" s="1" t="s">
@@ -30677,7 +30650,7 @@
       <c r="F820" s="1">
         <v>1</v>
       </c>
-      <c r="G820" s="14" t="s">
+      <c r="G820" s="1" t="s">
         <v>2043</v>
       </c>
       <c r="H820" s="1" t="s">
@@ -30758,7 +30731,7 @@
       <c r="F823" s="1">
         <v>0</v>
       </c>
-      <c r="G823" s="14" t="s">
+      <c r="G823" s="1" t="s">
         <v>2046</v>
       </c>
       <c r="H823" s="1" t="s">
@@ -30785,7 +30758,7 @@
       <c r="F824" s="1">
         <v>1</v>
       </c>
-      <c r="G824" s="14" t="s">
+      <c r="G824" s="1" t="s">
         <v>2047</v>
       </c>
       <c r="H824" s="1" t="s">
@@ -30812,7 +30785,7 @@
       <c r="F825" s="1">
         <v>1</v>
       </c>
-      <c r="G825" s="14" t="s">
+      <c r="G825" s="1" t="s">
         <v>2048</v>
       </c>
       <c r="H825" s="1" t="s">
@@ -30839,7 +30812,7 @@
       <c r="F826" s="1">
         <v>1</v>
       </c>
-      <c r="G826" s="14" t="s">
+      <c r="G826" s="1" t="s">
         <v>2049</v>
       </c>
       <c r="H826" s="1" t="s">
@@ -30893,7 +30866,7 @@
       <c r="F828" s="1">
         <v>1</v>
       </c>
-      <c r="G828" s="14" t="s">
+      <c r="G828" s="1" t="s">
         <v>2051</v>
       </c>
       <c r="H828" s="1" t="s">
@@ -30974,7 +30947,7 @@
       <c r="F831" s="1">
         <v>1</v>
       </c>
-      <c r="G831" s="14" t="s">
+      <c r="G831" s="1" t="s">
         <v>2054</v>
       </c>
       <c r="H831" s="1" t="s">
@@ -31001,7 +30974,7 @@
       <c r="F832" s="1">
         <v>1</v>
       </c>
-      <c r="G832" s="14" t="s">
+      <c r="G832" s="1" t="s">
         <v>2055</v>
       </c>
       <c r="H832" s="1" t="s">
@@ -31028,7 +31001,7 @@
       <c r="F833" s="1">
         <v>1</v>
       </c>
-      <c r="G833" s="14" t="s">
+      <c r="G833" s="1" t="s">
         <v>2056</v>
       </c>
       <c r="H833" s="1" t="s">
@@ -31082,7 +31055,7 @@
       <c r="F835" s="1">
         <v>1</v>
       </c>
-      <c r="G835" s="14" t="s">
+      <c r="G835" s="1" t="s">
         <v>2058</v>
       </c>
       <c r="H835" s="1" t="s">
@@ -31109,7 +31082,7 @@
       <c r="F836" s="1">
         <v>1</v>
       </c>
-      <c r="G836" s="14" t="s">
+      <c r="G836" s="1" t="s">
         <v>2059</v>
       </c>
       <c r="H836" s="1" t="s">
@@ -31244,7 +31217,7 @@
       <c r="F841" s="1">
         <v>1</v>
       </c>
-      <c r="G841" s="14" t="s">
+      <c r="G841" s="1" t="s">
         <v>2064</v>
       </c>
       <c r="H841" s="1" t="s">
@@ -31294,7 +31267,7 @@
       <c r="F843" s="1">
         <v>0</v>
       </c>
-      <c r="G843" s="14" t="s">
+      <c r="G843" s="1" t="s">
         <v>2065</v>
       </c>
       <c r="H843" s="1" t="s">
@@ -31429,7 +31402,7 @@
       <c r="F848" s="1">
         <v>1</v>
       </c>
-      <c r="G848" s="14" t="s">
+      <c r="G848" s="1" t="s">
         <v>2070</v>
       </c>
       <c r="H848" s="1" t="s">
@@ -31483,7 +31456,7 @@
       <c r="F850" s="1">
         <v>0</v>
       </c>
-      <c r="G850" s="14" t="s">
+      <c r="G850" s="1" t="s">
         <v>2072</v>
       </c>
       <c r="H850" s="1" t="s">
@@ -31510,7 +31483,7 @@
       <c r="F851" s="1">
         <v>0</v>
       </c>
-      <c r="G851" s="14" t="s">
+      <c r="G851" s="1" t="s">
         <v>2073</v>
       </c>
       <c r="H851" s="1" t="s">
@@ -31618,7 +31591,7 @@
       <c r="F855" s="1">
         <v>1</v>
       </c>
-      <c r="G855" s="14" t="s">
+      <c r="G855" s="1" t="s">
         <v>2077</v>
       </c>
       <c r="H855" s="1" t="s">
@@ -31699,7 +31672,7 @@
       <c r="F858" s="1">
         <v>1</v>
       </c>
-      <c r="G858" s="14" t="s">
+      <c r="G858" s="1" t="s">
         <v>2080</v>
       </c>
       <c r="H858" s="1" t="s">
@@ -33832,7 +33805,7 @@
       <c r="F937" s="1" t="s">
         <v>2313</v>
       </c>
-      <c r="G937" s="19" t="s">
+      <c r="G937" s="16" t="s">
         <v>2389</v>
       </c>
       <c r="H937" s="1" t="s">
@@ -34480,7 +34453,7 @@
       <c r="F961" s="1" t="s">
         <v>2313</v>
       </c>
-      <c r="G961" s="19" t="s">
+      <c r="G961" s="16" t="s">
         <v>2430</v>
       </c>
       <c r="H961" s="1" t="s">
@@ -35784,7 +35757,7 @@
       <c r="F1007" s="1">
         <v>1</v>
       </c>
-      <c r="G1007" s="14" t="s">
+      <c r="G1007" s="1" t="s">
         <v>2203</v>
       </c>
       <c r="H1007" s="1" t="s">
@@ -36248,7 +36221,7 @@
       <c r="F1023" s="1">
         <v>0</v>
       </c>
-      <c r="G1023" s="14" t="s">
+      <c r="G1023" s="1" t="s">
         <v>1433</v>
       </c>
       <c r="H1023" s="1" t="s">
@@ -36536,7 +36509,7 @@
       <c r="F1033" s="3">
         <v>0</v>
       </c>
-      <c r="G1033" s="16" t="s">
+      <c r="G1033" s="3" t="s">
         <v>1473</v>
       </c>
       <c r="H1033" s="3" t="s">
@@ -36681,7 +36654,7 @@
       <c r="F1038" s="1">
         <v>0</v>
       </c>
-      <c r="G1038" s="14" t="s">
+      <c r="G1038" s="1" t="s">
         <v>1518</v>
       </c>
       <c r="H1038" s="1" t="s">
@@ -36768,7 +36741,7 @@
       <c r="F1041" s="1">
         <v>0</v>
       </c>
-      <c r="G1041" s="14" t="s">
+      <c r="G1041" s="1" t="s">
         <v>1529</v>
       </c>
       <c r="H1041" s="1" t="s">
@@ -37261,7 +37234,7 @@
       <c r="F1058" s="1">
         <v>0</v>
       </c>
-      <c r="G1058" s="14" t="s">
+      <c r="G1058" s="1" t="s">
         <v>2234</v>
       </c>
       <c r="H1058" s="1" t="s">
@@ -37377,7 +37350,7 @@
       <c r="F1062" s="1">
         <v>1</v>
       </c>
-      <c r="G1062" s="14" t="s">
+      <c r="G1062" s="1" t="s">
         <v>1700</v>
       </c>
       <c r="H1062" s="1" t="s">
@@ -37812,7 +37785,7 @@
       <c r="F1077" s="1">
         <v>1</v>
       </c>
-      <c r="G1077" s="14" t="s">
+      <c r="G1077" s="1" t="s">
         <v>1751</v>
       </c>
       <c r="H1077" s="1" t="s">
@@ -38363,7 +38336,7 @@
       <c r="F1096" s="1">
         <v>0</v>
       </c>
-      <c r="G1096" s="14" t="s">
+      <c r="G1096" s="1" t="s">
         <v>2261</v>
       </c>
       <c r="H1096" s="1" t="s">
@@ -38421,7 +38394,7 @@
       <c r="F1098" s="1">
         <v>1</v>
       </c>
-      <c r="G1098" s="14" t="s">
+      <c r="G1098" s="1" t="s">
         <v>2263</v>
       </c>
       <c r="H1098" s="1" t="s">
@@ -38450,7 +38423,7 @@
       <c r="F1099" s="1">
         <v>1</v>
       </c>
-      <c r="G1099" s="14" t="s">
+      <c r="G1099" s="1" t="s">
         <v>2264</v>
       </c>
       <c r="H1099" s="1" t="s">
@@ -38941,7 +38914,7 @@
       <c r="F1116" s="1">
         <v>0</v>
       </c>
-      <c r="G1116" s="14" t="s">
+      <c r="G1116" s="1" t="s">
         <v>2270</v>
       </c>
       <c r="H1116" s="1" t="s">
@@ -39316,7 +39289,7 @@
       <c r="F1129" s="1">
         <v>1</v>
       </c>
-      <c r="G1129" s="14" t="s">
+      <c r="G1129" s="1" t="s">
         <v>2273</v>
       </c>
       <c r="H1129" s="1" t="s">
@@ -39358,7 +39331,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>